<commit_message>
best version: needs to fix ALU code for and or nor xor etc and LUI
</commit_message>
<xml_diff>
--- a/testcases_starter.xlsx
+++ b/testcases_starter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangyiming/Desktop/CMSC301Codes/Project_Checkpoint/Checkpoint2/cpu-processor-cmsc301/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33D8F23-7906-BB4D-BD16-575AF46D53E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D36094-E6AC-BC44-9275-8C576937495D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{35D5102D-44C0-204E-B01C-A98D67830E8C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Required setup</t>
   </si>
@@ -108,6 +108,21 @@
   </si>
   <si>
     <t># $s2 = 1 (because $t1 = 6 &lt; $t0 = 7)</t>
+  </si>
+  <si>
+    <t>addi $t2, $zero, 7</t>
+  </si>
+  <si>
+    <t>div $t2, $t0</t>
+  </si>
+  <si>
+    <t>Set $t2 to 7; set $t0 to 6</t>
+  </si>
+  <si>
+    <t># LO = 7 // 6 = 1, HI = 7 % 6 = 1</t>
+  </si>
+  <si>
+    <t>0x0148001a</t>
   </si>
 </sst>
 </file>
@@ -494,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DD8118-1B51-B941-9687-8518B9C0FED1}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,74 +537,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>